<commit_message>
Ghost Writer HTML - OK
</commit_message>
<xml_diff>
--- a/backend/Files/BooksWV.xlsx
+++ b/backend/Files/BooksWV.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APPS\SIMPLE\Parapreceptor\smart-article-aid\backend\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APPS\SIMPLE\Parapreceptor\Ghost_Writer_v1 (Html)\backend\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDD753A-137A-48BD-87FA-B754A10DE2AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1FD98E-36D1-4641-96B7-005F10212DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{8C43181E-41E2-4285-98AA-22B67AB52120}"/>
   </bookViews>
@@ -433,33 +433,6 @@
 vol. digital único (PDF); CCXL + 34.372 p.; 10a Ed. rev. e aum.; *Associação Internacional de Enciclopediologia Conscienciológica* (ENCYCLOSSAPIENS); &amp; *Associação Internacional Editares*; Foz do Iguaçu, PR; 2023</t>
   </si>
   <si>
-    <t>**Vieira**, Waldo; ***700 Experimentos da Conscienciologia***; 1.058 p.; 40 seções; 100 subseções; 700 caps.; 28,5 x 21,5 x 7 cm; enc.; Instituto Internacional de Projeciologia e Conscienciologia (IIPC); Rio de Janeiro, RJ; 1994</t>
-  </si>
-  <si>
-    <t>**Vieira**, Waldo; ***Conscienciograma: Técnica de Avaliação da Consciência Integral***; 344 p.; 150 abrevs.; 106 assuntos das folhas de avaliação; 21 x 14 cm; br.; Instituto Internacional de Projeciologia (IIP); Rio de Janeiro, RJ; 1996</t>
-  </si>
-  <si>
-    <t>**Vieira**, Waldo; ***Minidefinições Conscienciais***; 164 p.; 450 minifrases; 15 x 10 cm; br.; Instituto Internacional de Projeciologia (IIP); Rio de Janeiro, RJ; 1996</t>
-  </si>
-  <si>
-    <t>**Vieira**, Waldo; ***Homo sapiens pacificus***; 1.584 p.; 24 seções; 413 caps.; 29 x 21,5 x 7 cm; enc.; 3ª Ed. Gratuita; Centro de Altos Estudos da Conscienciologia (CEAEC); &amp; Associação Internacional Editares; Foz do Iguaçu, PR; 2007</t>
-  </si>
-  <si>
-    <t>**Vieira**, Waldo; ***Projeciologia: Panorama das Experiências da Consciência Fora do Corpo Humano***; 1.254 p.; 18 seções; 525 caps.; 28 x 21 x 7 cm; enc.; 10a Ed. rev. e aum.; Associação Internacional Editares; Foz do Iguaçu, PR; 2009</t>
-  </si>
-  <si>
-    <t>**Vieira**, Waldo; ***Manual da Proéxis: Programação Existencial***; 164 p.; 40 caps.; 21 x 14 cm; br.; 5ª Ed. Ver.; Associação Internacional Editares; Foz do Iguaçu, PR; 2011</t>
-  </si>
-  <si>
-    <t>**Vieira**, Waldo; ***Manual da Dupla Evolutiva***; 208 p.; 40 caps.; 21 x 14 cm; br.; 3ª Ed.; Associação Internacional Editares; Foz do Iguaçu, PR; 2012</t>
-  </si>
-  <si>
-    <t>**Vieira**, Waldo; ***700 Experimentos da Conscienciologia***;  1.088 p.; 40 seções; 100 subseções; 700 caps..; 28,5 x 21,5 x 7 cm; enc.; Associação Internacional Editares; Foz do Iguaçu, PR; 2013</t>
-  </si>
-  <si>
-    <t>**Vieira**, Waldo; ***Dicionário de Argumentos da Conscienciologia***; 1.572 p.;  651 caps.; 28,5 x 21,5 x 7 cm; enc.; Associação Internacional Editares; Foz do Iguaçu, PR; 2014</t>
-  </si>
-  <si>
     <t>**Vieira**, Waldo; ***Miniglossário da Conscienciologia***; 58 p.;  159 termos; 17 x 11 cm; br.; *Instituto Internacional de Projeciologia* (IIP); Rio de Janeiro, RJ; 1992</t>
   </si>
   <si>
@@ -509,6 +482,33 @@
   </si>
   <si>
     <t>**Vieira**, Waldo; ***200 Teáticas da Conscienciologia: Especialidades e Subcampos***;  260 p.; 200 caps.; 21 x 14 cm; br.; *Instituto Internacional de Projeciologia e Conscienciologia* (IIPC); Rio de Janeiro, RJ; 1997</t>
+  </si>
+  <si>
+    <t>**Vieira**, Waldo; ***Homo sapiens pacificus***; 1.584 p.; 24 seções; 413 caps.; 29 x 21,5 x 7 cm; enc.; 3ª Ed. Gratuita; *Centro de Altos Estudos da Conscienciologia* (CEAEC); &amp; *Associação Internacional Editares*; Foz do Iguaçu, PR; 2007</t>
+  </si>
+  <si>
+    <t>**Vieira**, Waldo; ***700 Experimentos da Conscienciologia***;  1.088 p.; 40 seções; 100 subseções; 700 caps..; 28,5 x 21,5 x 7 cm; enc.; *Associação Internacional Editares*; Foz do Iguaçu, PR; 2013</t>
+  </si>
+  <si>
+    <t>**Vieira**, Waldo; ***Dicionário de Argumentos da Conscienciologia***; 1.572 p.;  651 caps.; 28,5 x 21,5 x 7 cm; enc.; *Associação Internacional Editares*; Foz do Iguaçu, PR; 2014</t>
+  </si>
+  <si>
+    <t>**Vieira**, Waldo; ***Manual da Dupla Evolutiva***; 208 p.; 40 caps.; 21 x 14 cm; br.; 3ª Ed.; *Associação Internacional Editares*; Foz do Iguaçu, PR; 2012</t>
+  </si>
+  <si>
+    <t>**Vieira**, Waldo; ***Manual da Proéxis: Programação Existencial***; 164 p.; 40 caps.; 21 x 14 cm; br.; 5ª Ed. Ver.; *Associação Internacional Editares*; Foz do Iguaçu, PR; 2011</t>
+  </si>
+  <si>
+    <t>**Vieira**, Waldo; ***Projeciologia: Panorama das Experiências da Consciência Fora do Corpo Humano***; 1.254 p.; 18 seções; 525 caps.; 28 x 21 x 7 cm; enc.; 10a Ed. rev. e aum.; *Associação Internacional Editares*; Foz do Iguaçu, PR; 2009</t>
+  </si>
+  <si>
+    <t>**Vieira**, Waldo; ***Minidefinições Conscienciais***; 164 p.; 450 minifrases; 15 x 10 cm; br.; *Instituto Internacional de Projeciologia* (IIP); Rio de Janeiro, RJ; 1996</t>
+  </si>
+  <si>
+    <t>**Vieira**, Waldo; ***Conscienciograma: Técnica de Avaliação da Consciência Integral***; 344 p.; 150 abrevs.; 106 assuntos das folhas de avaliação; 21 x 14 cm; br.; *Instituto Internacional de Projeciologia* (IIP); Rio de Janeiro, RJ; 1996</t>
+  </si>
+  <si>
+    <t>**Vieira**, Waldo; ***700 Experimentos da Conscienciologia***; 1.058 p.; 40 seções; 100 subseções; 700 caps.; 28,5 x 21,5 x 7 cm; enc.; *Instituto Internacional de Projeciologia e Conscienciologia* (IIPC); Rio de Janeiro, RJ; 1994</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1100,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="16" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="K2" s="17" t="s">
         <v>53</v>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="16" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="K3" s="17" t="s">
         <v>9</v>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="16" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="K4" s="17" t="s">
         <v>14</v>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="16" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="K5" s="17" t="s">
         <v>16</v>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="16" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="K6" s="17" t="s">
         <v>48</v>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="16" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="K7" s="17" t="s">
         <v>50</v>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="16" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="K8" s="17" t="s">
         <v>4</v>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="16" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="K9" s="17" t="s">
         <v>6</v>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="16" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="K10" s="17" t="s">
         <v>68</v>
@@ -1474,7 +1474,7 @@
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="16" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="K11" s="17" t="s">
         <v>42</v>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="16" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="K12" s="17" t="s">
         <v>28</v>
@@ -1540,7 +1540,7 @@
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="16" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="K13" s="17" t="s">
         <v>65</v>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="16" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="K14" s="17" t="s">
         <v>25</v>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="16" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="K15" s="17" t="s">
         <v>45</v>
@@ -1639,7 +1639,7 @@
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="16" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="K16" s="17" t="s">
         <v>61</v>
@@ -1672,7 +1672,7 @@
       </c>
       <c r="I17" s="8"/>
       <c r="J17" s="16" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="K17" s="17" t="s">
         <v>56</v>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="I18" s="8"/>
       <c r="J18" s="16" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="K18" s="17" t="s">
         <v>37</v>
@@ -1738,7 +1738,7 @@
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="16" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="K19" s="17" t="s">
         <v>39</v>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="I20" s="8"/>
       <c r="J20" s="16" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="K20" s="17" t="s">
         <v>35</v>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="I21" s="8"/>
       <c r="J21" s="16" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="K21" s="17" t="s">
         <v>59</v>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="16" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="K22" s="17" t="s">
         <v>11</v>
@@ -1870,7 +1870,7 @@
       </c>
       <c r="I23" s="8"/>
       <c r="J23" s="16" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="K23" s="17" t="s">
         <v>63</v>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="I24" s="8"/>
       <c r="J24" s="16" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="K24" s="17" t="s">
         <v>19</v>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="I25" s="8"/>
       <c r="J25" s="16" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="K25" s="17" t="s">
         <v>22</v>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="I26" s="8"/>
       <c r="J26" s="16" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="K26" s="17" t="s">
         <v>30</v>
@@ -2002,7 +2002,7 @@
       </c>
       <c r="I27" s="14"/>
       <c r="J27" s="16" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="K27" s="18" t="s">
         <v>32</v>

</xml_diff>